<commit_message>
Delete DATE from profit
</commit_message>
<xml_diff>
--- a/public/template-rle-2.xlsx
+++ b/public/template-rle-2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">{name}</t>
   </si>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Конечный остаток</t>
   </si>
   <si>
-    <t xml:space="preserve">[date]</t>
+    <t xml:space="preserve">[title]</t>
   </si>
   <si>
     <t xml:space="preserve">[saldo_start]</t>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">[sum_accrual]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[sum_amount]</t>
   </si>
   <si>
     <t xml:space="preserve">[saldo_end]</t>
@@ -181,17 +178,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:G6"/>
+  <dimension ref="B3:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="11.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="11.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -202,7 +199,6 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
@@ -218,9 +214,6 @@
         <v>4</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -240,13 +233,10 @@
       <c r="F6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B3:F3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>